<commit_message>
PartsList spreadsheet update for Motor (SIDEWINDER)
</commit_message>
<xml_diff>
--- a/PartsList_RBG.xlsx
+++ b/PartsList_RBG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDCB051-F82D-4757-8C40-90B00E007FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1C5506-AD1D-4591-8AFE-9E6B38BE5044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="2625" windowWidth="20640" windowHeight="15360" xr2:uid="{08DBA8F4-1A8A-4F68-AF5D-84233C9FD0EF}"/>
+    <workbookView xWindow="1620" yWindow="1215" windowWidth="25200" windowHeight="17550" xr2:uid="{08DBA8F4-1A8A-4F68-AF5D-84233C9FD0EF}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsList" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Num</t>
   </si>
@@ -156,9 +164,6 @@
     <t>1K Ohm resistor, 1/4 watt (absolutely needed):</t>
   </si>
   <si>
-    <t>driver circuit for selenoid:</t>
-  </si>
-  <si>
     <t>small solenoid for rubber-band release coordinated with sound/light effects:</t>
   </si>
   <si>
@@ -193,6 +198,42 @@
   </si>
   <si>
     <t>https://smile.amazon.com/gp/product/B088H56DNY/ (expired)</t>
+  </si>
+  <si>
+    <t>driver circuit for selenoid (SILVER):</t>
+  </si>
+  <si>
+    <t>driver circuit for motor (SIDEWINDER):</t>
+  </si>
+  <si>
+    <t>Solenoid (SILVER) version</t>
+  </si>
+  <si>
+    <t>Mini Motor Low-speed Gearbox (4-speed) by Tamiya 70189**860.  assembled with 661.2:1 gear ratio</t>
+  </si>
+  <si>
+    <t>3.3V 800mA Linear Voltage Regulator - LD1117-3.3 TO-220.</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2165</t>
+  </si>
+  <si>
+    <t>Diode, 1N4001</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/755</t>
+  </si>
+  <si>
+    <t>https://www.robotshop.com/en/tamiya-4-speed-mini-gearbox-motor.html?gclid=CjwKCAjwjtOTBhAvEiwASG4bCAY395M_dBB8nr0g79zMdmdYRo1whBBhot3-KgAPBxbUhbIBIlP4YxoCVXIQAvD_BwE</t>
+  </si>
+  <si>
+    <t>Motor (SIDEWINDER) version</t>
+  </si>
+  <si>
+    <t>1K ohm 1/4 watt resistor</t>
+  </si>
+  <si>
+    <t>Base without firing mechanism</t>
   </si>
 </sst>
 </file>
@@ -570,15 +611,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212F0E84-C938-4091-ABFF-599F09C423F2}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G30" sqref="G30:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
     <col min="11" max="18" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -685,7 +727,7 @@
         <v>47.98</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -773,7 +815,7 @@
         <v>8.99</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -883,10 +925,10 @@
         <v>35.99</v>
       </c>
       <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -927,7 +969,7 @@
         <v>0.24</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
@@ -971,7 +1013,7 @@
         <v>0.2</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
@@ -1006,23 +1048,23 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G26" si="1">"| "&amp;A21&amp;" | $"&amp;TEXT(B21,"0.00")&amp;" | $"&amp;TEXT(C21,"0.00")&amp;" | "&amp;D21&amp;" | "&amp;E21&amp;" |"</f>
-        <v>| 0 | $0.00 | $0.00 | driver circuit for selenoid: | https://cdn-shop.adafruit.com/product-files/412/solenoid_driver.pdf |</v>
+        <f>"| "&amp;A21&amp;" | $"&amp;TEXT(B21,"0.00")&amp;" | $"&amp;TEXT(C21,"0.00")&amp;" | "&amp;D21&amp;" | "&amp;E21&amp;" |"</f>
+        <v>| 1 | $0.71 | $0.71 | USB 2.0 Breakout Board type A Female | https://www.amazon.com/Breakout-MELIFE-Adapter-2-54mm-Pinboard/dp/B07W7XMV3W |</v>
       </c>
       <c r="S21" s="2"/>
     </row>
@@ -1031,64 +1073,50 @@
         <v>1</v>
       </c>
       <c r="B22" s="1">
-        <v>14.29</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="C22" s="1">
-        <v>14.29</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>| 1 | $14.29 | $14.29 | small solenoid for rubber-band release coordinated with sound/light effects: | https://www.amazon.com/gp/product/B07TKTG3BH/ref=ox_sc_act_title_1?smid=A1THAZDOWP300U&amp;psc=1 |</v>
+        <f t="shared" ref="G22" si="1">"| "&amp;A22&amp;" | $"&amp;TEXT(B22,"0.00")&amp;" | $"&amp;TEXT(C22,"0.00")&amp;" | "&amp;D22&amp;" | "&amp;E22&amp;" |"</f>
+        <v>| 1 | $0.71 | $0.71 | USB 2.0 Breakout Board type A Male | https://www.amazon.com/MELIFE-Converter-2-54mm-Adapter-Breadboard/dp/B07W6T9KPJ |</v>
       </c>
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>| 1 | $0.83 | $0.83 | TIP120 Power Darlington Transistor: | https://www.adafruit.com/product/976 |</v>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="G23" t="s">
+        <v>6</v>
       </c>
       <c r="S23" s="2"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>| 1 | $0.10 | $0.10 | 1N4004 diode 1A 400V: | https://www.digikey.com/en/products/detail/nte-electronics-inc/1N4004/11645015 |</v>
+        <f t="shared" ref="G24:G28" si="2">"| "&amp;A24&amp;" | $"&amp;TEXT(B24,"0.00")&amp;" | $"&amp;TEXT(C24,"0.00")&amp;" | "&amp;D24&amp;" | "&amp;E24&amp;" |"</f>
+        <v>| 0 | $0.00 | $0.00 | driver circuit for selenoid (SILVER): | https://cdn-shop.adafruit.com/product-files/412/solenoid_driver.pdf |</v>
       </c>
       <c r="S24" s="2"/>
     </row>
@@ -1097,20 +1125,20 @@
         <v>1</v>
       </c>
       <c r="B25" s="1">
-        <v>0.1</v>
+        <v>14.29</v>
       </c>
       <c r="C25" s="1">
-        <v>0.1</v>
+        <v>14.29</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>| 1 | $0.10 | $0.10 | 2.2K Ohm resistor, 1/4 watt: | https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNMF14FTC2K20/2617325 |</v>
+        <f t="shared" si="2"/>
+        <v>| 1 | $14.29 | $14.29 | small solenoid for rubber-band release coordinated with sound/light effects: | https://www.amazon.com/gp/product/B07TKTG3BH/ref=ox_sc_act_title_1?smid=A1THAZDOWP300U&amp;psc=1 |</v>
       </c>
       <c r="S25" s="2"/>
     </row>
@@ -1119,20 +1147,20 @@
         <v>1</v>
       </c>
       <c r="B26" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C26" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="1"/>
-        <v>| 1 | $0.71 | $0.71 | USB 2.0 Breakout Board type A Female | https://www.amazon.com/Breakout-MELIFE-Adapter-2-54mm-Pinboard/dp/B07W7XMV3W |</v>
+        <f t="shared" si="2"/>
+        <v>| 1 | $0.83 | $0.83 | TIP120 Power Darlington Transistor: | https://www.adafruit.com/product/976 |</v>
       </c>
       <c r="S26" s="2"/>
     </row>
@@ -1141,49 +1169,237 @@
         <v>1</v>
       </c>
       <c r="B27" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="C27" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27" si="2">"| "&amp;A27&amp;" | $"&amp;TEXT(B27,"0.00")&amp;" | $"&amp;TEXT(C27,"0.00")&amp;" | "&amp;D27&amp;" | "&amp;E27&amp;" |"</f>
-        <v>| 1 | $0.71 | $0.71 | USB 2.0 Breakout Board type A Male | https://www.amazon.com/MELIFE-Converter-2-54mm-Adapter-Breadboard/dp/B07W6T9KPJ |</v>
+        <f t="shared" si="2"/>
+        <v>| 1 | $0.10 | $0.10 | 1N4004 diode 1A 400V: | https://www.digikey.com/en/products/detail/nte-electronics-inc/1N4004/11645015 |</v>
       </c>
       <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>| 1 | $0.10 | $0.10 | 2.2K Ohm resistor, 1/4 watt: | https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNMF14FTC2K20/2617325 |</v>
+      </c>
       <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
       <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" ref="G30:G34" si="3">"| "&amp;A30&amp;" | $"&amp;TEXT(B30,"0.00")&amp;" | $"&amp;TEXT(C30,"0.00")&amp;" | "&amp;D30&amp;" | "&amp;E30&amp;" |"</f>
+        <v>| 0 | $0.00 | $0.00 | driver circuit for motor (SIDEWINDER): |  |</v>
+      </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C31" s="4">
-        <f>SUM(C3:C30)</f>
-        <v>133.36733333333331</v>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <v>9.86</v>
+      </c>
+      <c r="C31" s="1">
+        <v>9.86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="3"/>
+        <v>| 1 | $9.86 | $9.86 | Mini Motor Low-speed Gearbox (4-speed) by Tamiya 70189**860.  assembled with 661.2:1 gear ratio | https://www.robotshop.com/en/tamiya-4-speed-mini-gearbox-motor.html?gclid=CjwKCAjwjtOTBhAvEiwASG4bCAY395M_dBB8nr0g79zMdmdYRo1whBBhot3-KgAPBxbUhbIBIlP4YxoCVXIQAvD_BwE |</v>
+      </c>
+      <c r="S31" s="2"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="3"/>
+        <v>| 1 | $1.25 | $1.25 | 3.3V 800mA Linear Voltage Regulator - LD1117-3.3 TO-220. | https://www.adafruit.com/product/2165 |</v>
+      </c>
+      <c r="S32" s="2"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>| 1 | $0.15 | $0.15 | Diode, 1N4001 | https://www.adafruit.com/product/755 |</v>
+      </c>
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>| 1 | $0.84 | $0.84 | 1K ohm 1/4 watt resistor | https://www.digikey.com/en/products/detail/ohmite/OD102JE/823687 |</v>
+      </c>
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="S35" s="2"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="S36" s="2"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1">
+        <f>SUM(C3:C24)</f>
+        <v>118.044</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="S38" s="2"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1">
+        <f>SUM(C25:C28)</f>
+        <v>15.323333333333332</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S39" s="2"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1">
+        <f>SUM(C30:C34)</f>
+        <v>12.1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="S40" s="2"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="S41" s="2"/>
+    </row>
+    <row r="42" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C42" s="4">
+        <f>SUM(C3:C28)</f>
+        <v>133.36733333333333</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C43" s="4">
+        <f>SUM(C3:C24)+SUM(C30:C34)</f>
+        <v>130.14400000000001</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E15" r:id="rId1" xr:uid="{4179C11A-EB86-4F61-ABD6-E6DC52A52262}"/>
+    <hyperlink ref="E32" r:id="rId2" xr:uid="{B7848707-0C39-4285-BC8E-F17E731E973F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>